<commit_message>
Added performance tests plan
</commit_message>
<xml_diff>
--- a/PlanTestow.xlsx
+++ b/PlanTestow.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\KUBA\PROJECTS\TestujSystell\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F4491B9-E9BD-49BB-9ABC-1EFCD3591791}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2292DEC-F266-44AD-9F05-731C76706E49}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
   <si>
     <t>Testy jednostkowe</t>
   </si>
@@ -70,6 +70,15 @@
   </si>
   <si>
     <t>Zmiana języka na angielski działa</t>
+  </si>
+  <si>
+    <t>Testy wydajnościowe</t>
+  </si>
+  <si>
+    <t>Dziesięciokrotna nawigacja do "https://systell.pl/blog/" z wszystkimi czasami poniżej 3 sekund</t>
+  </si>
+  <si>
+    <t>Dziesięciokrotne wejście na stronę główną oraz kliknięcie w link "Więcej postów"</t>
   </si>
 </sst>
 </file>
@@ -532,10 +541,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:F16"/>
+  <dimension ref="B2:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -641,8 +650,37 @@
         <v>12</v>
       </c>
     </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B17" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" s="10"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="10"/>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C18" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" s="12"/>
+      <c r="E18" s="12"/>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D19" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E19" s="8"/>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E20" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="12">
+    <mergeCell ref="B17:E17"/>
+    <mergeCell ref="C18:E18"/>
+    <mergeCell ref="D19:E19"/>
     <mergeCell ref="D13:E13"/>
     <mergeCell ref="D11:E11"/>
     <mergeCell ref="D15:E15"/>

</xml_diff>

<commit_message>
Finished all unit tests for main site
</commit_message>
<xml_diff>
--- a/PlanTestow.xlsx
+++ b/PlanTestow.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PROJECTS\TestujSystell\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E672BC69-A802-4D33-9842-B1E82568B96B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7F8E752-2AC5-465E-9DB6-36CF9FE4D8A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="19440" windowHeight="15150" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -239,16 +239,16 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="1" xfId="3" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="49" fontId="4" fillId="5" borderId="4" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="4" borderId="1" xfId="3" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="3" borderId="3" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -543,8 +543,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -558,19 +558,19 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.3">
       <c r="D4" s="11" t="s">
@@ -611,11 +611,11 @@
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.3">
       <c r="D11" s="11" t="s">
@@ -652,19 +652,19 @@
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B17" s="9" t="s">
+      <c r="B17" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="10"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="10"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="C18" s="7" t="s">
+      <c r="C18" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="10"/>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.3">
       <c r="D19" s="11" t="s">
@@ -679,18 +679,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="D8:E8"/>
     <mergeCell ref="B17:E17"/>
     <mergeCell ref="C18:E18"/>
     <mergeCell ref="D19:E19"/>
     <mergeCell ref="D13:E13"/>
     <mergeCell ref="D11:E11"/>
     <mergeCell ref="D15:E15"/>
-    <mergeCell ref="C10:E10"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="D8:E8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated privacy test login
</commit_message>
<xml_diff>
--- a/PlanTestow.xlsx
+++ b/PlanTestow.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PROJECTS\TestujSystell\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7F8E752-2AC5-465E-9DB6-36CF9FE4D8A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E963C003-A35F-4DDE-B061-9424DC0D6852}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,9 +39,6 @@
     <t>Fragment RODO po angielsku znajduje się na stronie: "agree to be contacted via telephone or email in order to be provided with commercial offers of Systell"</t>
   </si>
   <si>
-    <t>Przejście na stronę "https://systell.pl/polityka-prywatnosci/"</t>
-  </si>
-  <si>
     <t>Strona aktualności "https://systell.pl/aktualnosci/"</t>
   </si>
   <si>
@@ -66,9 +63,6 @@
     <t>W kodzie html strony znajduje się "&lt;title&gt;Aktualności&lt;/title&gt;"</t>
   </si>
   <si>
-    <t>Link polityki prywatności działa poprawnie</t>
-  </si>
-  <si>
     <t>Zmiana języka na angielski działa</t>
   </si>
   <si>
@@ -79,6 +73,12 @@
   </si>
   <si>
     <t>Dziesięciokrotne wejście w tej samej chwili na stronę główną oraz kliknięcie w link "Więcej postów"</t>
+  </si>
+  <si>
+    <t>Link polityki prywatności ma poprawny odnośnik</t>
+  </si>
+  <si>
+    <t>Odnośnik "polityka prywatności" zawiera odniesienie do "polityka-prywatnosci"</t>
   </si>
 </sst>
 </file>
@@ -239,16 +239,16 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="4" fillId="5" borderId="4" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="49" fontId="3" fillId="4" borderId="1" xfId="3" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="5" borderId="4" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="3" borderId="3" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -544,7 +544,7 @@
   <dimension ref="B2:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -558,19 +558,19 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C3" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
+      <c r="C3" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.3">
       <c r="D4" s="11" t="s">
@@ -588,7 +588,7 @@
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.3">
       <c r="D6" s="11" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E6" s="12"/>
     </row>
@@ -601,96 +601,96 @@
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.3">
       <c r="D8" s="11" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="E8" s="12"/>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.3">
       <c r="E9" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C10" s="7" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C10" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.3">
       <c r="D11" s="11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E11" s="12"/>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.3">
       <c r="D12" s="2"/>
       <c r="E12" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.3">
       <c r="D13" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E13" s="12"/>
     </row>
     <row r="14" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="E14" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.3">
       <c r="D15" s="11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E15" s="12"/>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.3">
       <c r="E16" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B17" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
+      <c r="B17" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C17" s="10"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="10"/>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="C18" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="D18" s="10"/>
-      <c r="E18" s="10"/>
+      <c r="C18" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18" s="8"/>
+      <c r="E18" s="8"/>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.3">
       <c r="D19" s="11" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E19" s="12"/>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.3">
       <c r="E20" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="B17:E17"/>
+    <mergeCell ref="C18:E18"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="D15:E15"/>
     <mergeCell ref="C10:E10"/>
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="C3:E3"/>
     <mergeCell ref="D4:E4"/>
     <mergeCell ref="D6:E6"/>
     <mergeCell ref="D8:E8"/>
-    <mergeCell ref="B17:E17"/>
-    <mergeCell ref="C18:E18"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="D15:E15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Finished performance tests and added numeration to test plan file
</commit_message>
<xml_diff>
--- a/PlanTestow.xlsx
+++ b/PlanTestow.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PROJECTS\TestujSystell\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E963C003-A35F-4DDE-B061-9424DC0D6852}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCA7E2F8-4EB6-454C-983C-F9EE78F4D6EC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
   <si>
     <t>Testy jednostkowe</t>
   </si>
@@ -69,9 +69,6 @@
     <t>Testy wydajnościowe</t>
   </si>
   <si>
-    <t>Dziesięciokrotna nawigacja do "https://systell.pl/blog/" z wszystkimi czasami poniżej 3 sekund</t>
-  </si>
-  <si>
     <t>Dziesięciokrotne wejście w tej samej chwili na stronę główną oraz kliknięcie w link "Więcej postów"</t>
   </si>
   <si>
@@ -79,13 +76,55 @@
   </si>
   <si>
     <t>Odnośnik "polityka prywatności" zawiera odniesienie do "polityka-prywatnosci"</t>
+  </si>
+  <si>
+    <t>W</t>
+  </si>
+  <si>
+    <t>J</t>
+  </si>
+  <si>
+    <t>J.1</t>
+  </si>
+  <si>
+    <t>J.2</t>
+  </si>
+  <si>
+    <t>W.1</t>
+  </si>
+  <si>
+    <t>J.1.1</t>
+  </si>
+  <si>
+    <t>J.1.2</t>
+  </si>
+  <si>
+    <t>J.1.3</t>
+  </si>
+  <si>
+    <t>J.2.1</t>
+  </si>
+  <si>
+    <t>J.2.2</t>
+  </si>
+  <si>
+    <t>J.2.3</t>
+  </si>
+  <si>
+    <t>W.1.1</t>
+  </si>
+  <si>
+    <t>DODATKOWE WYMAGANIA MASZYNY TESTOWEJ: średni PING na "https://systell.pl/" &lt;= 6ms oraz RAM &gt;= 8GM</t>
+  </si>
+  <si>
+    <t>Dziesięciokrotna nawigacja do "https://systell.pl/blog/" z wszystkimi czasami poniżej 5 sekund</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -126,8 +165,29 @@
       <charset val="238"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -154,8 +214,25 @@
         <fgColor rgb="FFA5A5A5"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -202,68 +279,79 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1" shrinkToFit="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="5" borderId="4" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="6" borderId="0" xfId="6" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="8" borderId="0" xfId="8" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="7" borderId="0" xfId="7" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="5" borderId="2" xfId="4" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="4" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="4" borderId="1" xfId="3" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="3" borderId="3" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="5" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="9">
+    <cellStyle name="20% - Accent1" xfId="7" builtinId="30"/>
+    <cellStyle name="60% - Accent1" xfId="8" builtinId="32"/>
+    <cellStyle name="Accent1" xfId="6" builtinId="29"/>
     <cellStyle name="Check Cell" xfId="4" builtinId="23"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Input" xfId="3" builtinId="20"/>
     <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Warning Text" xfId="5" builtinId="11"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -541,156 +629,198 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:F20"/>
+  <dimension ref="B2:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="1"/>
-    <col min="2" max="2" width="8" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10.88671875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="27.5546875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="86" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.109375" style="1"/>
+    <col min="1" max="2" width="9.109375" style="1"/>
+    <col min="3" max="3" width="11.6640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="40.88671875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="27.5546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="86" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B2" s="9" t="s">
+    <row r="2" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-    </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C3" s="7" t="s">
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+    </row>
+    <row r="3" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="D4" s="11" t="s">
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+    </row>
+    <row r="4" spans="2:7" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="12"/>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="3" t="s">
+      <c r="F4" s="15"/>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="E5" s="2"/>
+      <c r="F5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F5" s="2"/>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="D6" s="11" t="s">
+      <c r="G5" s="2"/>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B6" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="12"/>
-    </row>
-    <row r="7" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="4" t="s">
+      <c r="F6" s="15"/>
+    </row>
+    <row r="7" spans="2:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="E7" s="2"/>
+      <c r="F7" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="D8" s="11" t="s">
+    <row r="8" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B8" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8" s="15"/>
+    </row>
+    <row r="9" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F9" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="E8" s="12"/>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="E9" s="5" t="s">
+    </row>
+    <row r="10" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B10" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+    </row>
+    <row r="11" spans="2:7" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="F11" s="15"/>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="E12" s="2"/>
+      <c r="F12" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B13" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E13" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="F13" s="15"/>
+    </row>
+    <row r="14" spans="2:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="F14" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B15" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="E15" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="F15" s="15"/>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="F16" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B17" s="7" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C10" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="D11" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="E11" s="12"/>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="D12" s="2"/>
-      <c r="E12" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="D13" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="E13" s="12"/>
-    </row>
-    <row r="14" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="E14" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="D15" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="E15" s="12"/>
-    </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="E16" s="6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B17" s="9" t="s">
+      <c r="C17" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="C17" s="10"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="10"/>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="C18" s="7" t="s">
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+    </row>
+    <row r="18" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B18" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="D19" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="E19" s="12"/>
-    </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="E20" s="3" t="s">
+      <c r="D18" s="11"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
+    </row>
+    <row r="19" spans="2:6" ht="33" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C19" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="D19" s="16"/>
+      <c r="E19" s="14" t="s">
         <v>14</v>
       </c>
+      <c r="F19" s="15"/>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="F20" s="3" t="s">
+        <v>30</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="12">
-    <mergeCell ref="B17:E17"/>
-    <mergeCell ref="C18:E18"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="C10:E10"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="D8:E8"/>
+  <mergeCells count="13">
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="C3:F3"/>
+    <mergeCell ref="C10:F10"/>
+    <mergeCell ref="C17:F17"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C18:F18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Fixed typos in test plan
</commit_message>
<xml_diff>
--- a/PlanTestow.xlsx
+++ b/PlanTestow.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PROJECTS\TestujSystell\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\KUBA\PROJECTS\TestujSystell\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCA7E2F8-4EB6-454C-983C-F9EE78F4D6EC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D021127B-A049-4166-B1B3-7F410AA7D2EC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -114,10 +114,10 @@
     <t>W.1.1</t>
   </si>
   <si>
-    <t>DODATKOWE WYMAGANIA MASZYNY TESTOWEJ: średni PING na "https://systell.pl/" &lt;= 6ms oraz RAM &gt;= 8GM</t>
-  </si>
-  <si>
     <t>Dziesięciokrotna nawigacja do "https://systell.pl/blog/" z wszystkimi czasami poniżej 5 sekund</t>
+  </si>
+  <si>
+    <t>DODATKOWE WYMAGANIA MASZYNY TESTOWEJ: średni PING na "https://systell.pl/" &lt;= 6ms oraz RAM &gt;= 8GB</t>
   </si>
 </sst>
 </file>
@@ -320,22 +320,22 @@
     <xf numFmtId="49" fontId="5" fillId="7" borderId="0" xfId="7" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="1" xfId="3" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="3" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="4" fillId="5" borderId="2" xfId="4" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="4" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="4" borderId="1" xfId="3" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="3" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="5" applyAlignment="1">
@@ -632,187 +632,182 @@
   <dimension ref="B2:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="9.109375" style="1"/>
-    <col min="3" max="3" width="11.6640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="40.88671875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="27.5546875" style="1" customWidth="1"/>
+    <col min="1" max="2" width="9.140625" style="1"/>
+    <col min="3" max="3" width="11.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="40.85546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="27.5703125" style="1" customWidth="1"/>
     <col min="6" max="6" width="86" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.109375" style="1"/>
+    <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-    </row>
-    <row r="3" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+    </row>
+    <row r="3" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-    </row>
-    <row r="4" spans="2:7" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+    </row>
+    <row r="4" spans="2:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B4" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="E4" s="14" t="s">
+      <c r="E4" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="F4" s="15"/>
-    </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="F4" s="13"/>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="E5" s="2"/>
       <c r="F5" s="3" t="s">
         <v>2</v>
       </c>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="E6" s="14" t="s">
+      <c r="E6" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="F6" s="15"/>
-    </row>
-    <row r="7" spans="2:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="F6" s="13"/>
+    </row>
+    <row r="7" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="E7" s="2"/>
       <c r="F7" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B8" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="E8" s="14" t="s">
+      <c r="E8" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="F8" s="15"/>
-    </row>
-    <row r="9" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F8" s="13"/>
+    </row>
+    <row r="9" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F9" s="5" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="C10" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-    </row>
-    <row r="11" spans="2:7" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="D10" s="15"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="15"/>
+    </row>
+    <row r="11" spans="2:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B11" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="E11" s="14" t="s">
+      <c r="E11" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="F11" s="15"/>
-    </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="F11" s="13"/>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
       <c r="E12" s="2"/>
       <c r="F12" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B13" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="E13" s="14" t="s">
+      <c r="E13" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="F13" s="15"/>
-    </row>
-    <row r="14" spans="2:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="F13" s="13"/>
+    </row>
+    <row r="14" spans="2:7" ht="45" x14ac:dyDescent="0.25">
       <c r="F14" s="6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B15" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="E15" s="14" t="s">
+      <c r="E15" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="F15" s="15"/>
-    </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="F15" s="13"/>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F16" s="6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="12" t="s">
+      <c r="C17" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="D17" s="13"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
-    </row>
-    <row r="18" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D17" s="11"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
+    </row>
+    <row r="18" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="C18" s="10" t="s">
+      <c r="C18" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="D18" s="11"/>
-      <c r="E18" s="11"/>
-      <c r="F18" s="11"/>
-    </row>
-    <row r="19" spans="2:6" ht="33" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="D18" s="15"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="15"/>
+    </row>
+    <row r="19" spans="2:6" ht="33" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B19" s="9" t="s">
         <v>28</v>
       </c>
       <c r="C19" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="D19" s="16"/>
+      <c r="E19" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="F19" s="13"/>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F20" s="3" t="s">
         <v>29</v>
-      </c>
-      <c r="D19" s="16"/>
-      <c r="E19" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="F19" s="15"/>
-    </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="F20" s="3" t="s">
-        <v>30</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="C2:F2"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="C3:F3"/>
     <mergeCell ref="C10:F10"/>
     <mergeCell ref="C17:F17"/>
     <mergeCell ref="E19:F19"/>
@@ -821,6 +816,11 @@
     <mergeCell ref="E15:F15"/>
     <mergeCell ref="C19:D19"/>
     <mergeCell ref="C18:F18"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="C3:F3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Created test results file
</commit_message>
<xml_diff>
--- a/PlanTestow.xlsx
+++ b/PlanTestow.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\KUBA\PROJECTS\TestujSystell\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D021127B-A049-4166-B1B3-7F410AA7D2EC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F5C6E6C-7F1A-4729-BD90-4D2CE4C392D3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
   <si>
     <t>Testy jednostkowe</t>
   </si>
@@ -66,9 +66,6 @@
     <t>Zmiana języka na angielski działa</t>
   </si>
   <si>
-    <t>Testy wydajnościowe</t>
-  </si>
-  <si>
     <t>Dziesięciokrotne wejście w tej samej chwili na stronę główną oraz kliknięcie w link "Więcej postów"</t>
   </si>
   <si>
@@ -117,7 +114,7 @@
     <t>Dziesięciokrotna nawigacja do "https://systell.pl/blog/" z wszystkimi czasami poniżej 5 sekund</t>
   </si>
   <si>
-    <t>DODATKOWE WYMAGANIA MASZYNY TESTOWEJ: średni PING na "https://systell.pl/" &lt;= 6ms oraz RAM &gt;= 8GB</t>
+    <t>Testy wydajnościowe i obciążeniowe</t>
   </si>
 </sst>
 </file>
@@ -632,14 +629,14 @@
   <dimension ref="B2:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="9.140625" style="1"/>
     <col min="3" max="3" width="11.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="40.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="19.5703125" style="1" customWidth="1"/>
     <col min="5" max="5" width="27.5703125" style="1" customWidth="1"/>
     <col min="6" max="6" width="86" style="1" customWidth="1"/>
     <col min="7" max="16384" width="9.140625" style="1"/>
@@ -647,7 +644,7 @@
   <sheetData>
     <row r="2" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C2" s="10" t="s">
         <v>0</v>
@@ -658,7 +655,7 @@
     </row>
     <row r="3" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C3" s="14" t="s">
         <v>5</v>
@@ -669,7 +666,7 @@
     </row>
     <row r="4" spans="2:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B4" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E4" s="12" t="s">
         <v>1</v>
@@ -685,7 +682,7 @@
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E6" s="12" t="s">
         <v>12</v>
@@ -700,21 +697,21 @@
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B8" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F8" s="13"/>
     </row>
     <row r="9" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F9" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C10" s="14" t="s">
         <v>4</v>
@@ -725,7 +722,7 @@
     </row>
     <row r="11" spans="2:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B11" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E11" s="12" t="s">
         <v>8</v>
@@ -740,21 +737,21 @@
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B13" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E13" s="12" t="s">
         <v>6</v>
       </c>
       <c r="F13" s="13"/>
     </row>
-    <row r="14" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:7" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F14" s="6" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B15" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E15" s="12" t="s">
         <v>10</v>
@@ -768,10 +765,10 @@
     </row>
     <row r="17" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="D17" s="11"/>
       <c r="E17" s="11"/>
@@ -779,7 +776,7 @@
     </row>
     <row r="18" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C18" s="14" t="s">
         <v>5</v>
@@ -790,20 +787,18 @@
     </row>
     <row r="19" spans="2:6" ht="33" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B19" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="C19" s="16" t="s">
-        <v>30</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="C19" s="16"/>
       <c r="D19" s="16"/>
       <c r="E19" s="12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F19" s="13"/>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.25">
       <c r="F20" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>